<commit_message>
added SPs and page
</commit_message>
<xml_diff>
--- a/docs/docs/extension-timelimit.xlsx
+++ b/docs/docs/extension-timelimit.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="75">
   <si>
     <t>Path</t>
   </si>
@@ -134,13 +134,19 @@
     <t>0</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Questions and answer time limit</t>
+  </si>
+  <si>
+    <t>A duration associated with completion of a Questionnaire or Questionnaire item.  This is used to determine if the end user has completed the Questionnaire or individual questions or groups of questions within the specified time-period.</t>
+  </si>
+  <si>
+    <t>To determine whether the questionnaire or items were answered within the time limit defined by the extension, the Form Filler can record the start and stop date-times in the [Argonaut QuestionnaireResponse responsePeriod Extension]. How this information modifies the behavior of the Form-filler or interpretation of results is an implementation detail outside of scope of this Implementation Guide.</t>
+  </si>
+  <si>
     <t>*</t>
-  </si>
-  <si>
-    <t>Optional Extensions Element</t>
-  </si>
-  <si>
-    <t>Optional Extension Element - found in all resources.</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1
@@ -148,16 +154,10 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>N/A</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>Extension.id</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t xml:space="preserve">string {[]} {[]}
@@ -225,7 +225,10 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://fhir.org/guides/argonaut-questionnaire/StructureDefinition/extension-limit"/&gt;</t>
+    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://fhir.org/guides/argonaut-questionnaire/StructureDefinition/extension-timeLimit"/&gt;</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
   <si>
     <t>Extension.valueDuration</t>
@@ -583,7 +586,9 @@
       <c r="L2" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="M2" s="2"/>
+      <c r="M2" t="s" s="2">
+        <v>42</v>
+      </c>
       <c r="N2" s="2"/>
       <c r="O2" t="s" s="2">
         <v>37</v>
@@ -638,21 +643,21 @@
         <v>38</v>
       </c>
       <c r="AG2" t="s" s="2">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -663,7 +668,7 @@
         <v>38</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G3" t="s" s="2">
         <v>37</v>
@@ -738,7 +743,7 @@
         <v>38</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AH3" t="s" s="2">
         <v>37</v>
@@ -763,7 +768,7 @@
         <v>38</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s" s="2">
         <v>37</v>
@@ -840,7 +845,7 @@
         <v>38</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="AH4" t="s" s="2">
         <v>37</v>
@@ -862,10 +867,10 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>37</v>
@@ -939,10 +944,10 @@
         <v>62</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>37</v>
@@ -951,15 +956,15 @@
         <v>37</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s" s="2">
         <v>37</v>
@@ -969,7 +974,7 @@
         <v>38</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>37</v>
@@ -981,13 +986,13 @@
         <v>37</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1038,13 +1043,13 @@
         <v>37</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>38</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>37</v>
@@ -1053,7 +1058,7 @@
         <v>37</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>